<commit_message>
Pulled Hellbred and Fey'ri calculations off the CreatureInfo sheet
</commit_message>
<xml_diff>
--- a/data/CreatureInfo.xlsx
+++ b/data/CreatureInfo.xlsx
@@ -20,20 +20,12 @@
   <definedNames>
     <definedName name="CustomRace">'[1]Custom Race'!$D$3:$D$47</definedName>
     <definedName name="DragonbornAspect">'[1]Race &amp; Templates'!$P$4</definedName>
-    <definedName name="DragonwroughtSkill">[1]Tables!$I$273</definedName>
-    <definedName name="FeyriDR">'[1]Race &amp; Templates'!$AZ$19</definedName>
-    <definedName name="FeyriHasSpecialAbility">'[1]Race &amp; Templates'!$AG$12</definedName>
-    <definedName name="FtDarkBlood">[1]Feats!$AR$2629</definedName>
-    <definedName name="FtDragonwrought">[1]Feats!$AR$1323</definedName>
     <definedName name="FtEpicDragonWildShape">[1]Feats!$AR$3460</definedName>
     <definedName name="FtWaterAdaptation">[1]Feats!$AR$1459</definedName>
     <definedName name="Gender">'[1]Race &amp; Templates'!$AG$3</definedName>
     <definedName name="HasTemplate">'[1]Template Info'!$AP$1</definedName>
-    <definedName name="HellbredAspect">'[1]Race &amp; Templates'!$P$7</definedName>
     <definedName name="HitDice">'[1]Class Info'!$EF$8</definedName>
-    <definedName name="HRCA">[1]ExportSheet!$B$31</definedName>
     <definedName name="HRDLCS">[1]ExportSheet!$B$105</definedName>
-    <definedName name="HRLivingGreyhawk">[1]ExportSheet!$B$110</definedName>
     <definedName name="IsLycanthropeAlternate">Sheet1!$CT$63</definedName>
     <definedName name="RaceNA">'[1]Race Info'!$M$1</definedName>
     <definedName name="RegionTxt">'[1]Race &amp; Templates'!$D$11</definedName>
@@ -51,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6970" uniqueCount="1878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6983" uniqueCount="1888">
   <si>
     <t>Short Description</t>
   </si>
@@ -5687,6 +5679,36 @@
   </si>
   <si>
     <t>Hengeyokai</t>
+  </si>
+  <si>
+    <t>ref:KoboldSkills</t>
+  </si>
+  <si>
+    <t>Bhuka, Goblin, Giant</t>
+  </si>
+  <si>
+    <t>Sylvan, Elven</t>
+  </si>
+  <si>
+    <t>ref:FeyriDRValue</t>
+  </si>
+  <si>
+    <t>ref:FeyriLA</t>
+  </si>
+  <si>
+    <t>ref:HellbredDarkvision</t>
+  </si>
+  <si>
+    <t>ref:HellbredConAdj</t>
+  </si>
+  <si>
+    <t>ref:HellbredIntAdj</t>
+  </si>
+  <si>
+    <t>ref:HellbredChaAdj</t>
+  </si>
+  <si>
+    <t>ref:HellbredSkills</t>
   </si>
 </sst>
 </file>
@@ -5934,11 +5956,6 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="31">
-          <cell r="B31" t="b">
-            <v>0</v>
-          </cell>
-        </row>
         <row r="77">
           <cell r="W77">
             <v>1</v>
@@ -5949,15 +5966,10 @@
             <v>0</v>
           </cell>
         </row>
-        <row r="110">
-          <cell r="B110" t="b">
-            <v>0</v>
-          </cell>
-        </row>
       </sheetData>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4">
         <row r="31">
           <cell r="M31" t="str">
@@ -5975,28 +5987,18 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
       <sheetData sheetId="11"/>
-      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="12"/>
       <sheetData sheetId="13">
         <row r="3">
           <cell r="AG3" t="str">
             <v/>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="AG12" t="b">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="AZ19" t="b">
-            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -6152,7 +6154,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="15"/>
       <sheetData sheetId="16">
         <row r="8">
           <cell r="EF8">
@@ -6160,37 +6162,27 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
       <sheetData sheetId="35">
-        <row r="1323">
-          <cell r="AR1323" t="b">
-            <v>0</v>
-          </cell>
-        </row>
         <row r="1459">
           <cell r="AR1459" t="b">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="2629">
-          <cell r="AR2629" t="b">
             <v>0</v>
           </cell>
         </row>
@@ -6200,41 +6192,35 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
       <sheetData sheetId="49"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
-      <sheetData sheetId="59" refreshError="1"/>
-      <sheetData sheetId="60" refreshError="1"/>
-      <sheetData sheetId="61" refreshError="1"/>
-      <sheetData sheetId="62" refreshError="1"/>
-      <sheetData sheetId="63" refreshError="1"/>
-      <sheetData sheetId="64">
-        <row r="273">
-          <cell r="I273" t="str">
-            <v>None</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
+      <sheetData sheetId="53"/>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
+      <sheetData sheetId="59"/>
+      <sheetData sheetId="60"/>
+      <sheetData sheetId="61"/>
+      <sheetData sheetId="62"/>
+      <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6507,10 +6493,10 @@
   <dimension ref="A1:BO518"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M321" sqref="M321"/>
+      <selection pane="bottomRight" activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8003,9 +7989,8 @@
       <c r="AT12" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="AU12" s="5" t="str">
-        <f>IF(HRLivingGreyhawk,"Flan, Goblin, Giant","Bhuka, Goblin, Giant")</f>
-        <v>Bhuka, Goblin, Giant</v>
+      <c r="AU12" s="5" t="s">
+        <v>1879</v>
       </c>
       <c r="AV12" s="5"/>
       <c r="AW12" s="7"/>
@@ -10195,9 +10180,8 @@
         <v>1800</v>
       </c>
       <c r="AS32" s="5"/>
-      <c r="AT32" s="5" t="str">
-        <f>IF(HRLivingGreyhawk,"Common, Giant",IF(HRDLCS,"Common, Sylvan","Sylvan,Elven"))</f>
-        <v>Sylvan,Elven</v>
+      <c r="AT32" s="5" t="s">
+        <v>1880</v>
       </c>
       <c r="AU32" s="5" t="str">
         <f>IF(HRDLCS,"Abanasinian, Elven, Goblin, Ogre","Common, Gnome, Halfling")</f>
@@ -18308,9 +18292,8 @@
         <v>45</v>
       </c>
       <c r="Y108" s="5"/>
-      <c r="Z108" s="5" t="str">
-        <f>IF(FeyriDR,"10/magic","")</f>
-        <v/>
+      <c r="Z108" s="5" t="s">
+        <v>1881</v>
       </c>
       <c r="AA108" s="5"/>
       <c r="AB108" s="5"/>
@@ -18347,9 +18330,8 @@
       </c>
       <c r="AV108" s="5"/>
       <c r="AW108" s="7"/>
-      <c r="AX108" s="5">
-        <f>2+FeyriHasSpecialAbility</f>
-        <v>2</v>
+      <c r="AX108" s="5" t="s">
+        <v>1882</v>
       </c>
       <c r="AY108" s="5" t="s">
         <v>318</v>
@@ -25971,9 +25953,8 @@
       <c r="Q180" s="5"/>
       <c r="R180" s="5"/>
       <c r="S180" s="5"/>
-      <c r="T180" s="5">
-        <f>IF(HellbredAspect="Spirit (Su)",30+30*(HitDice&gt;=6)+60*(HitDice&gt;=9),0)</f>
-        <v>0</v>
+      <c r="T180" s="5" t="s">
+        <v>1883</v>
       </c>
       <c r="U180" s="7"/>
       <c r="V180" s="5"/>
@@ -25992,22 +25973,18 @@
       <c r="AI180" s="5"/>
       <c r="AJ180" s="5"/>
       <c r="AK180" s="5"/>
-      <c r="AL180" s="5">
-        <f>IF(HellbredAspect="Body (Ex)",2,IF(HellbredAspect="Spirit (Su)",-2,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AM180" s="5">
-        <f>IF(HellbredAspect="Body (Ex)",-2,0)</f>
-        <v>0</v>
+      <c r="AL180" s="5" t="s">
+        <v>1884</v>
+      </c>
+      <c r="AM180" s="5" t="s">
+        <v>1885</v>
       </c>
       <c r="AN180" s="5"/>
-      <c r="AO180" s="5">
-        <f>IF(HellbredAspect="Spirit (Su)",2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AP180" s="5" t="str">
-        <f>"Intimidate+2"&amp;IF(HellbredAspect="Spirit (Su)",",Sense Motive+2","")</f>
-        <v>Intimidate+2</v>
+      <c r="AO180" s="5" t="s">
+        <v>1886</v>
+      </c>
+      <c r="AP180" s="5" t="s">
+        <v>1887</v>
       </c>
       <c r="AQ180" s="5"/>
       <c r="AR180" s="5"/>
@@ -27960,13 +27937,11 @@
       <c r="C199" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D199" s="5" t="str">
-        <f>IF(FtDragonwrought,"Dragon","Humanoid")</f>
-        <v>Humanoid</v>
-      </c>
-      <c r="E199" s="5" t="str">
-        <f>IF(FtDragonwrought,"Reptilian","Dragonblood, Reptilian")</f>
-        <v>Dragonblood, Reptilian</v>
+      <c r="D199" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E199" s="5" t="s">
+        <v>849</v>
       </c>
       <c r="F199" s="5"/>
       <c r="G199" s="5">
@@ -28040,9 +28015,8 @@
       <c r="AO199" s="5">
         <v>0</v>
       </c>
-      <c r="AP199" s="5" t="str">
-        <f>IF(FtDragonwrought,DragonwroughtSkill &amp; "+2,","")&amp;"Craft (trapmaking)+2,Profession (miner)+2,Search+2"</f>
-        <v>Craft (trapmaking)+2,Profession (miner)+2,Search+2</v>
+      <c r="AP199" s="5" t="s">
+        <v>1878</v>
       </c>
       <c r="AQ199" s="5"/>
       <c r="AR199" s="5"/>

</xml_diff>

<commit_message>
Made lycanthropes work with the new datasheet format
</commit_message>
<xml_diff>
--- a/data/CreatureInfo.xlsx
+++ b/data/CreatureInfo.xlsx
@@ -24,8 +24,6 @@
     <definedName name="HasTemplate">'[1]Template Info'!$AP$1</definedName>
     <definedName name="HitDice">'[1]Class Info'!$EF$8</definedName>
     <definedName name="HRDLCS">[1]ExportSheet!$B$105</definedName>
-    <definedName name="IsLycanthropeAlternate">Sheet1!$CU$63</definedName>
-    <definedName name="RaceNA">'[1]Race Info'!$M$1</definedName>
     <definedName name="RegionTxt">'[1]Race &amp; Templates'!$D$11</definedName>
     <definedName name="TblRaceInfo">Sheet1!$A$3:$BN$319</definedName>
     <definedName name="TinkerGnomeGuild">'[1]Race &amp; Templates'!$P$14</definedName>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7223" uniqueCount="1874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7179" uniqueCount="1874">
   <si>
     <t>Short Description</t>
   </si>
@@ -5969,7 +5967,7 @@
       <sheetData sheetId="16">
         <row r="8">
           <cell r="EF8">
-            <v>9</v>
+            <v>10</v>
           </cell>
         </row>
       </sheetData>
@@ -6293,10 +6291,10 @@
   <dimension ref="A1:BP522"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C173" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J294" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J198" sqref="J198"/>
+      <selection pane="bottomRight" activeCell="M317" sqref="M317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -41244,8 +41242,7 @@
       <c r="L321" s="5"/>
       <c r="M321" s="5"/>
       <c r="N321" s="5">
-        <f>2+IF(IsLycanthropeAlternate, MAX(5,RaceNA),0)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O321" s="5" t="s">
         <v>1249</v>
@@ -41643,8 +41640,7 @@
       <c r="L325" s="5"/>
       <c r="M325" s="5"/>
       <c r="N325" s="5">
-        <f>2+IF(IsLycanthropeAlternate, MAX(6,RaceNA),0)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O325" s="5" t="s">
         <v>1255</v>
@@ -60952,7 +60948,6 @@
       <c r="L518" s="5"/>
       <c r="M518" s="5"/>
       <c r="N518" s="5">
-        <f>2+IF(IsLycanthropeAlternate, MAX(2,RaceNA),0)</f>
         <v>2</v>
       </c>
       <c r="O518" s="5" t="s">

</xml_diff>